<commit_message>
email search, forgot APIs
</commit_message>
<xml_diff>
--- a/uploads/sample.xlsx
+++ b/uploads/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2E7DFF-E7CF-488D-AC36-773298049600}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D096784D-7A45-4B63-A22A-EEA2E213D6C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{927E4CEA-9580-EB42-8777-2CC6D9B95D54}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="56">
   <si>
     <t>Food Item</t>
   </si>
@@ -190,9 +190,6 @@
   </si>
   <si>
     <t>sea</t>
-  </si>
-  <si>
-    <t>baker</t>
   </si>
   <si>
     <t>continental</t>
@@ -347,7 +344,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -359,7 +356,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -687,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09399BBD-75D3-6B4C-9C16-AC9FA597ECF8}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16:H25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -701,7 +698,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="16" t="s">
         <v>28</v>
       </c>
       <c r="B1" s="17" t="s">
@@ -711,13 +708,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="19"/>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="16" t="s">
         <v>51</v>
       </c>
       <c r="H1" s="7" t="s">
@@ -737,7 +734,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="18"/>
       <c r="C2" s="1" t="s">
         <v>27</v>
@@ -745,9 +742,9 @@
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
@@ -755,7 +752,7 @@
       <c r="L2" s="7"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+      <c r="A3" s="12">
         <v>1</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -793,7 +790,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="14"/>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -811,7 +808,7 @@
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="14"/>
       <c r="C5" s="2" t="s">
         <v>14</v>
@@ -829,7 +826,7 @@
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="14"/>
       <c r="C6" s="2" t="s">
         <v>5</v>
@@ -847,7 +844,7 @@
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="12"/>
       <c r="B7" s="14"/>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -865,7 +862,7 @@
       <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="14"/>
       <c r="C8" s="2" t="s">
         <v>8</v>
@@ -883,7 +880,7 @@
       <c r="L8" s="9"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="14"/>
       <c r="C9" s="2" t="s">
         <v>9</v>
@@ -901,7 +898,7 @@
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="14"/>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -919,7 +916,7 @@
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="14"/>
       <c r="C11" s="2" t="s">
         <v>11</v>
@@ -937,7 +934,7 @@
       <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="14"/>
       <c r="C12" s="2" t="s">
         <v>12</v>
@@ -955,7 +952,7 @@
       <c r="L12" s="9"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="14"/>
       <c r="C13" s="2" t="s">
         <v>13</v>
@@ -973,7 +970,7 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="14"/>
       <c r="C14" s="2" t="s">
         <v>24</v>
@@ -991,7 +988,7 @@
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="15"/>
       <c r="C15" s="2" t="s">
         <v>25</v>
@@ -1028,7 +1025,7 @@
         <v>40</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>29</v>
@@ -1209,10 +1206,10 @@
       <c r="L25" s="10"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="16">
+      <c r="A26" s="12">
         <v>3</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="12" t="s">
         <v>44</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -1221,14 +1218,14 @@
       <c r="D26" s="2">
         <v>52</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="F26" s="16" t="s">
+      <c r="F26" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G26" s="16" t="s">
-        <v>56</v>
+      <c r="G26" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="H26" s="11" t="s">
         <v>29</v>
@@ -1247,17 +1244,17 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
       <c r="H27" s="11"/>
       <c r="I27" s="11"/>
       <c r="J27" s="11"/>
@@ -1265,17 +1262,17 @@
       <c r="L27" s="11"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
       <c r="H28" s="11"/>
       <c r="I28" s="11"/>
       <c r="J28" s="11"/>
@@ -1283,17 +1280,17 @@
       <c r="L28" s="11"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
       <c r="J29" s="11"/>
@@ -1301,17 +1298,17 @@
       <c r="L29" s="11"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
       <c r="H30" s="11"/>
       <c r="I30" s="11"/>
       <c r="J30" s="11"/>
@@ -1319,17 +1316,17 @@
       <c r="L30" s="11"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
-      <c r="B31" s="16"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
       <c r="H31" s="11"/>
       <c r="I31" s="11"/>
       <c r="J31" s="11"/>
@@ -1337,17 +1334,17 @@
       <c r="L31" s="11"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="16"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
       <c r="J32" s="11"/>
@@ -1355,17 +1352,17 @@
       <c r="L32" s="11"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="16"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
       <c r="H33" s="11"/>
       <c r="I33" s="11"/>
       <c r="J33" s="11"/>
@@ -1373,17 +1370,17 @@
       <c r="L33" s="11"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="16"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D34" s="3">
         <v>0.06</v>
       </c>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
       <c r="H34" s="11"/>
       <c r="I34" s="11"/>
       <c r="J34" s="11"/>
@@ -1391,17 +1388,17 @@
       <c r="L34" s="11"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
-      <c r="B35" s="16"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D35" s="3">
         <v>0.24</v>
       </c>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
       <c r="H35" s="11"/>
       <c r="I35" s="11"/>
       <c r="J35" s="11"/>

</xml_diff>